<commit_message>
Modify the Excel file and split test_cdpa.py
</commit_message>
<xml_diff>
--- a/docs/cdpa_stats.xlsx
+++ b/docs/cdpa_stats.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yaaco\Documents\FortifyIQ\Github\cdpa\cdpa-any-order\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yaaco\Documents\FortifyIQ\Github\cdpa\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F2F0BD-FC90-4E31-9B36-146CD19DBF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9839CB2B-F91D-448D-A120-AE77009245F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{CA994CFE-64CA-40BE-8708-C616CF713A40}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{CA994CFE-64CA-40BE-8708-C616CF713A40}"/>
   </bookViews>
   <sheets>
     <sheet name="bit" sheetId="1" r:id="rId1"/>
     <sheet name="lsb" sheetId="2" r:id="rId2"/>
     <sheet name="res" sheetId="3" r:id="rId3"/>
+    <sheet name="chart" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -423,17 +424,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -485,6 +476,1460 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Noise 0</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="11"/>
+              <c:pt idx="0">
+                <c:v>128</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>256</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>512</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1024</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>2048</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>131072</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>res!$E$3:$O$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.5859375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.734375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>89.55078125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.90234375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-99AD-4C58-9608-E79DD1512E56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Noise 4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="11"/>
+              <c:pt idx="0">
+                <c:v>128</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>256</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>512</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1024</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>2048</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>131072</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>res!$E$4:$O$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.765625E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.58984375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.54296875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96.484375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-99AD-4C58-9608-E79DD1512E56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Noise 8</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="11"/>
+              <c:pt idx="0">
+                <c:v>128</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>256</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>512</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1024</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>2048</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>131072</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>res!$E$5:$O$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.390625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.13671875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>81.0546875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99.51171875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-99AD-4C58-9608-E79DD1512E56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Noise 16</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="11"/>
+              <c:pt idx="0">
+                <c:v>128</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>256</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>512</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1024</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>2048</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>131072</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>res!$E$6:$O$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48828125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.58203125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85.25390625</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>99.8046875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-99AD-4C58-9608-E79DD1512E56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Noise 32</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="11"/>
+              <c:pt idx="0">
+                <c:v>128</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>256</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>512</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1024</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>2048</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>131072</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>res!$E$7:$O$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.48828125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.78125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>86.9140625</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>99.609375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-99AD-4C58-9608-E79DD1512E56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="329441680"/>
+        <c:axId val="329434608"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="329441680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t># of traces</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="329434608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="329434608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t>Success</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" baseline="0"/>
+                  <a:t> rate</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1800"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="329441680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{6540DF66-9CE9-408A-BD19-C34712D548B6}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8661797" cy="6290469"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F77EC66B-EC2B-067A-4AA5-DC7C2C9523CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1740,7 +3185,7 @@
     <mergeCell ref="B23:B26"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:R27">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1753,7 +3198,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
@@ -2684,7 +4129,7 @@
     <mergeCell ref="B14:B15"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:R27">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>65</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2696,11 +4141,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{997663CD-D5C0-484A-BB5C-91215F844F0A}">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3628,10 +5073,10 @@
     <mergeCell ref="B14:B15"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:R27">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>45</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Change the copyright. Minor changes in cdpa_stats.xlsx
</commit_message>
<xml_diff>
--- a/docs/cdpa_stats.xlsx
+++ b/docs/cdpa_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yaaco\Documents\FortifyIQ\Github\cdpa\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56C67EB-5520-463E-95DE-8591BF4C568F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC89D395-55BF-486D-A12A-FF73B5D5FC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{CA994CFE-64CA-40BE-8708-C616CF713A40}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{CA994CFE-64CA-40BE-8708-C616CF713A40}"/>
   </bookViews>
   <sheets>
     <sheet name="bit" sheetId="1" r:id="rId1"/>
@@ -387,6 +387,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -394,6 +399,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -412,14 +420,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1046,7 +1046,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1059,8 +1059,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1800"/>
-                  <a:t># of traces</a:t>
+                  <a:rPr lang="en-US" sz="2800"/>
+                  <a:t># of simulated 32-bit CDPA traces</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1078,7 +1078,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1167,7 +1167,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1180,14 +1180,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:rPr lang="en-US" sz="2800"/>
                   <a:t>Success</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1800" baseline="0"/>
-                  <a:t> rate</a:t>
+                  <a:rPr lang="en-US" sz="2800" baseline="0"/>
+                  <a:t> rate (in %)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1800"/>
+                <a:endParaRPr lang="en-US" sz="2800"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1204,7 +1204,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1893,7 +1893,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{6540DF66-9CE9-408A-BD19-C34712D548B6}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="64" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2249,23 +2249,23 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="27"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="30"/>
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
@@ -2324,10 +2324,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="28">
+      <c r="A3" s="31">
         <v>32</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="34">
         <v>1</v>
       </c>
       <c r="C3" s="5">
@@ -2336,16 +2336,16 @@
       <c r="D3" s="23">
         <v>63.28125</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3" s="26">
         <v>76.932973710317398</v>
       </c>
-      <c r="F3" s="35">
+      <c r="F3" s="26">
         <v>92.9036458333333</v>
       </c>
-      <c r="G3" s="35">
+      <c r="G3" s="26">
         <v>99.167596726190396</v>
       </c>
-      <c r="H3" s="35">
+      <c r="H3" s="26">
         <v>100</v>
       </c>
       <c r="I3" s="13"/>
@@ -2360,215 +2360,215 @@
       <c r="R3" s="14"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="28"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="3">
         <v>4</v>
       </c>
       <c r="D4" s="23">
         <v>53.241257440476097</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="26">
         <v>58.5720486111111</v>
       </c>
-      <c r="F4" s="35">
+      <c r="F4" s="26">
         <v>67.7951388888888</v>
       </c>
-      <c r="G4" s="35">
+      <c r="G4" s="26">
         <v>83.770461309523796</v>
       </c>
-      <c r="H4" s="35">
+      <c r="H4" s="26">
         <v>96.360367063492006</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="26">
         <v>99.874441964285694</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4" s="26">
         <v>100</v>
       </c>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
       <c r="R4" s="15"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="28"/>
-      <c r="B5" s="31"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="3">
         <v>8</v>
       </c>
       <c r="D5" s="23"/>
-      <c r="E5" s="35">
+      <c r="E5" s="26">
         <v>52.0724826388888</v>
       </c>
-      <c r="F5" s="35">
+      <c r="F5" s="26">
         <v>55.222284226190403</v>
       </c>
-      <c r="G5" s="35">
+      <c r="G5" s="26">
         <v>61.638144841269799</v>
       </c>
-      <c r="H5" s="35">
+      <c r="H5" s="26">
         <v>73.465401785714207</v>
       </c>
-      <c r="I5" s="35">
+      <c r="I5" s="26">
         <v>89.504278273809504</v>
       </c>
-      <c r="J5" s="35">
+      <c r="J5" s="26">
         <v>98.7738715277777</v>
       </c>
-      <c r="K5" s="35">
+      <c r="K5" s="26">
         <v>99.975198412698404</v>
       </c>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
       <c r="R5" s="15"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="28"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="3">
         <v>16</v>
       </c>
       <c r="D6" s="23"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35">
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26">
         <v>52.743675595238003</v>
       </c>
-      <c r="H6" s="35">
+      <c r="H6" s="26">
         <v>56.096540178571402</v>
       </c>
-      <c r="I6" s="35">
+      <c r="I6" s="26">
         <v>62.580605158730101</v>
       </c>
-      <c r="J6" s="35">
+      <c r="J6" s="26">
         <v>75.9114583333333</v>
       </c>
-      <c r="K6" s="35">
+      <c r="K6" s="26">
         <v>91.404699900793602</v>
       </c>
-      <c r="L6" s="35">
+      <c r="L6" s="26">
         <v>99.063740079365004</v>
       </c>
-      <c r="M6" s="35">
+      <c r="M6" s="26">
         <v>99.964347718253904</v>
       </c>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
       <c r="R6" s="15"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="28"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="3">
         <v>32</v>
       </c>
       <c r="D7" s="23"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35">
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26">
         <v>51.316034226190403</v>
       </c>
-      <c r="I7" s="35">
+      <c r="I7" s="26">
         <v>52.988591269841201</v>
       </c>
-      <c r="J7" s="35">
+      <c r="J7" s="26">
         <v>55.8051215277777</v>
       </c>
-      <c r="K7" s="35">
+      <c r="K7" s="26">
         <v>63.121589781746003</v>
       </c>
-      <c r="L7" s="35">
+      <c r="L7" s="26">
         <v>76.221478174603106</v>
       </c>
-      <c r="M7" s="35">
+      <c r="M7" s="26">
         <v>91.745721726190396</v>
       </c>
-      <c r="N7" s="35">
+      <c r="N7" s="26">
         <v>99.141245039682502</v>
       </c>
-      <c r="O7" s="35">
+      <c r="O7" s="26">
         <v>99.995349702380906</v>
       </c>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
       <c r="R7" s="15"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="28"/>
-      <c r="B8" s="31"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="3">
         <v>64</v>
       </c>
       <c r="D8" s="23"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35">
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26">
         <v>52.377852182539598</v>
       </c>
-      <c r="L8" s="35">
+      <c r="L8" s="26">
         <v>55.843874007936499</v>
       </c>
-      <c r="M8" s="35">
+      <c r="M8" s="26">
         <v>62.885974702380899</v>
       </c>
-      <c r="N8" s="35">
+      <c r="N8" s="26">
         <v>75.680493551587304</v>
       </c>
-      <c r="O8" s="35">
+      <c r="O8" s="26">
         <v>91.660466269841194</v>
       </c>
-      <c r="P8" s="35">
+      <c r="P8" s="26">
         <v>99.040488591269806</v>
       </c>
-      <c r="Q8" s="35">
+      <c r="Q8" s="26">
         <v>100</v>
       </c>
       <c r="R8" s="15"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="28"/>
-      <c r="B9" s="32"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="10">
         <v>128</v>
       </c>
       <c r="D9" s="23"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35">
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26">
         <v>52.611917162698397</v>
       </c>
-      <c r="N9" s="35">
+      <c r="N9" s="26">
         <v>55.955481150793602</v>
       </c>
-      <c r="O9" s="35">
+      <c r="O9" s="26">
         <v>62.603856646825299</v>
       </c>
-      <c r="P9" s="35">
+      <c r="P9" s="26">
         <v>75.403025793650698</v>
       </c>
-      <c r="Q9" s="35">
+      <c r="Q9" s="26">
         <v>91.951884920634896</v>
       </c>
       <c r="R9" s="15">
@@ -2576,8 +2576,8 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="28"/>
-      <c r="B10" s="33">
+      <c r="A10" s="31"/>
+      <c r="B10" s="37">
         <v>2</v>
       </c>
       <c r="C10" s="12">
@@ -2614,71 +2614,71 @@
       <c r="R10" s="16"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="28"/>
-      <c r="B11" s="31"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="3">
         <v>4</v>
       </c>
       <c r="D11" s="23"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35">
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26">
         <v>53.0490451388888</v>
       </c>
-      <c r="K11" s="35">
+      <c r="K11" s="26">
         <v>56.226748511904702</v>
       </c>
-      <c r="L11" s="35">
+      <c r="L11" s="26">
         <v>62.741815476190403</v>
       </c>
-      <c r="M11" s="35">
+      <c r="M11" s="26">
         <v>76.145523313492006</v>
       </c>
-      <c r="N11" s="35">
+      <c r="N11" s="26">
         <v>91.8402777777777</v>
       </c>
-      <c r="O11" s="35">
+      <c r="O11" s="26">
         <v>99.156746031745996</v>
       </c>
-      <c r="P11" s="35">
+      <c r="P11" s="26">
         <v>99.990699404761898</v>
       </c>
-      <c r="Q11" s="35"/>
+      <c r="Q11" s="26"/>
       <c r="R11" s="15"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="28"/>
-      <c r="B12" s="31"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="3">
         <v>8</v>
       </c>
       <c r="D12" s="23"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35">
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26">
         <v>51.621403769841201</v>
       </c>
-      <c r="M12" s="35">
+      <c r="M12" s="26">
         <v>53.644283234126902</v>
       </c>
-      <c r="N12" s="35">
+      <c r="N12" s="26">
         <v>57.781498015872998</v>
       </c>
-      <c r="O12" s="35">
+      <c r="O12" s="26">
         <v>66.381448412698404</v>
       </c>
-      <c r="P12" s="35">
+      <c r="P12" s="26">
         <v>82.265314980158706</v>
       </c>
-      <c r="Q12" s="35">
+      <c r="Q12" s="26">
         <v>95.760478670634896</v>
       </c>
       <c r="R12" s="15">
@@ -2686,8 +2686,8 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
-      <c r="B13" s="32"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="10">
         <v>16</v>
       </c>
@@ -2714,33 +2714,33 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="28"/>
-      <c r="B14" s="31">
+      <c r="A14" s="31"/>
+      <c r="B14" s="35">
         <v>3</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
       </c>
       <c r="D14" s="23"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35">
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26">
         <v>52.242993551587297</v>
       </c>
-      <c r="O14" s="35">
+      <c r="O14" s="26">
         <v>55.367993551587297</v>
       </c>
-      <c r="P14" s="35">
+      <c r="P14" s="26">
         <v>61.921812996031697</v>
       </c>
-      <c r="Q14" s="35">
+      <c r="Q14" s="26">
         <v>73.680865575396794</v>
       </c>
       <c r="R14" s="15">
@@ -2748,27 +2748,27 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="28"/>
-      <c r="B15" s="31"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="3">
         <v>4</v>
       </c>
       <c r="D15" s="23"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35">
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26">
         <v>52.129836309523803</v>
       </c>
-      <c r="Q15" s="35">
+      <c r="Q15" s="26">
         <v>54.682849702380899</v>
       </c>
       <c r="R15" s="15">
@@ -2776,10 +2776,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="38">
+      <c r="A16" s="32">
         <v>64</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="34">
         <v>1</v>
       </c>
       <c r="C16" s="5">
@@ -2814,176 +2814,176 @@
       <c r="R16" s="14"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17" s="28"/>
-      <c r="B17" s="31"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="3">
         <v>4</v>
       </c>
       <c r="D17" s="23"/>
-      <c r="E17" s="35">
+      <c r="E17" s="26">
         <v>55.660986712598401</v>
       </c>
-      <c r="F17" s="35">
+      <c r="F17" s="26">
         <v>62.881397637795203</v>
       </c>
-      <c r="G17" s="35">
+      <c r="G17" s="26">
         <v>76.087290846456696</v>
       </c>
-      <c r="H17" s="35">
+      <c r="H17" s="26">
         <v>92.148283710629897</v>
       </c>
-      <c r="I17" s="35">
+      <c r="I17" s="26">
         <v>99.1703063484252</v>
       </c>
-      <c r="J17" s="35">
+      <c r="J17" s="26">
         <v>99.995386318897602</v>
       </c>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
       <c r="R17" s="15"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18" s="28"/>
-      <c r="B18" s="31"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="3">
         <v>8</v>
       </c>
       <c r="D18" s="23"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35">
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26">
         <v>59.7425565944881</v>
       </c>
-      <c r="H18" s="35">
+      <c r="H18" s="26">
         <v>71.053764763779498</v>
       </c>
-      <c r="I18" s="35">
+      <c r="I18" s="26">
         <v>87.033249261810994</v>
       </c>
-      <c r="J18" s="35">
+      <c r="J18" s="26">
         <v>98.016117125984195</v>
       </c>
-      <c r="K18" s="35">
+      <c r="K18" s="26">
         <v>99.930025836614107</v>
       </c>
-      <c r="L18" s="35">
+      <c r="L18" s="26">
         <v>100</v>
       </c>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="26"/>
       <c r="R18" s="15"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A19" s="28"/>
-      <c r="B19" s="31"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="3">
         <v>16</v>
       </c>
       <c r="D19" s="23"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35">
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26">
         <v>61.096671998031397</v>
       </c>
-      <c r="J19" s="35">
+      <c r="J19" s="26">
         <v>74.076494832677099</v>
       </c>
-      <c r="K19" s="35">
+      <c r="K19" s="26">
         <v>90.324341781496003</v>
       </c>
-      <c r="L19" s="35">
+      <c r="L19" s="26">
         <v>98.808132381889706</v>
       </c>
-      <c r="M19" s="35">
+      <c r="M19" s="26">
         <v>99.987696850393704</v>
       </c>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
       <c r="R19" s="15"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A20" s="28"/>
-      <c r="B20" s="31"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="3">
         <v>32</v>
       </c>
       <c r="D20" s="23"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35">
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26">
         <v>55.4218442421259</v>
       </c>
-      <c r="K20" s="35">
+      <c r="K20" s="26">
         <v>62.705308809055097</v>
       </c>
-      <c r="L20" s="35">
+      <c r="L20" s="26">
         <v>75.348332923228298</v>
       </c>
-      <c r="M20" s="35">
+      <c r="M20" s="26">
         <v>91.380105807086593</v>
       </c>
-      <c r="N20" s="35">
+      <c r="N20" s="26">
         <v>99.034971702755897</v>
       </c>
-      <c r="O20" s="35">
+      <c r="O20" s="26">
         <v>99.993848425196802</v>
       </c>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="26"/>
       <c r="R20" s="15"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A21" s="28"/>
-      <c r="B21" s="31"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="3">
         <v>64</v>
       </c>
       <c r="D21" s="23"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35">
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26">
         <v>55.594857283464499</v>
       </c>
-      <c r="M21" s="35">
+      <c r="M21" s="26">
         <v>62.7691313976378</v>
       </c>
-      <c r="N21" s="35">
+      <c r="N21" s="26">
         <v>76.1249692421259</v>
       </c>
-      <c r="O21" s="35">
+      <c r="O21" s="26">
         <v>91.619248277558995</v>
       </c>
-      <c r="P21" s="35">
+      <c r="P21" s="26">
         <v>99.131090059055097</v>
       </c>
-      <c r="Q21" s="35">
+      <c r="Q21" s="26">
         <v>99.986927903543304</v>
       </c>
       <c r="R21" s="15"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A22" s="28"/>
-      <c r="B22" s="32"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="10">
         <v>128</v>
       </c>
@@ -3014,97 +3014,97 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A23" s="28"/>
-      <c r="B23" s="31">
+      <c r="A23" s="31"/>
+      <c r="B23" s="35">
         <v>2</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
       </c>
       <c r="D23" s="23"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35">
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26">
         <v>55.9070497047244</v>
       </c>
-      <c r="L23" s="35">
+      <c r="L23" s="26">
         <v>62.9390686515748</v>
       </c>
-      <c r="M23" s="35">
+      <c r="M23" s="26">
         <v>75.999630905511793</v>
       </c>
-      <c r="N23" s="35">
+      <c r="N23" s="26">
         <v>91.576187253936993</v>
       </c>
-      <c r="O23" s="35">
+      <c r="O23" s="26">
         <v>99.195681594488093</v>
       </c>
-      <c r="P23" s="35">
+      <c r="P23" s="26">
         <v>99.987696850393704</v>
       </c>
-      <c r="Q23" s="35"/>
+      <c r="Q23" s="26"/>
       <c r="R23" s="15"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
-      <c r="B24" s="31"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="3">
         <v>4</v>
       </c>
       <c r="D24" s="23"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35">
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26">
         <v>60.892901082677099</v>
       </c>
-      <c r="N24" s="35">
+      <c r="N24" s="26">
         <v>72.995355561023601</v>
       </c>
-      <c r="O24" s="35">
+      <c r="O24" s="26">
         <v>89.280880905511793</v>
       </c>
-      <c r="P24" s="35">
+      <c r="P24" s="26">
         <v>98.571296751968504</v>
       </c>
-      <c r="Q24" s="35">
+      <c r="Q24" s="26">
         <v>99.967704232283396</v>
       </c>
       <c r="R24" s="15"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A25" s="28"/>
-      <c r="B25" s="31"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="3">
         <v>8</v>
       </c>
       <c r="D25" s="23"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="35">
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26">
         <v>60.899052657480297</v>
       </c>
-      <c r="P25" s="35">
+      <c r="P25" s="26">
         <v>72.604730561023601</v>
       </c>
-      <c r="Q25" s="35">
+      <c r="Q25" s="26">
         <v>89.486958661417304</v>
       </c>
       <c r="R25" s="15">
@@ -3112,12 +3112,12 @@
       </c>
     </row>
     <row r="26" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="29"/>
-      <c r="B26" s="34"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="38"/>
       <c r="C26" s="4">
         <v>16</v>
       </c>
-      <c r="D26" s="37"/>
+      <c r="D26" s="27"/>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
       <c r="G26" s="21"/>
@@ -3159,7 +3159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1CBE5AC-06A3-496E-A1F3-E257F37237CD}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3175,23 +3175,23 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="27"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="30"/>
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
@@ -3250,10 +3250,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="38">
+      <c r="A3" s="32">
         <v>32</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="34">
         <v>1</v>
       </c>
       <c r="C3" s="5">
@@ -3286,215 +3286,215 @@
       <c r="R3" s="14"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="28"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="3">
         <v>4</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="26">
         <v>2.96630859375</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="26">
         <v>4.98046875</v>
       </c>
-      <c r="F4" s="35">
+      <c r="F4" s="26">
         <v>9.1949462890625</v>
       </c>
-      <c r="G4" s="35">
+      <c r="G4" s="26">
         <v>27.9754638671875</v>
       </c>
-      <c r="H4" s="35">
+      <c r="H4" s="26">
         <v>72.7996826171875</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="26">
         <v>98.7335205078125</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4" s="26">
         <v>100</v>
       </c>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
       <c r="R4" s="15"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="28"/>
-      <c r="B5" s="31"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="3">
         <v>8</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35">
+      <c r="D5" s="26"/>
+      <c r="E5" s="26">
         <v>2.2979736328125</v>
       </c>
-      <c r="F5" s="35">
+      <c r="F5" s="26">
         <v>3.485107421875</v>
       </c>
-      <c r="G5" s="35">
+      <c r="G5" s="26">
         <v>6.04248046875</v>
       </c>
-      <c r="H5" s="35">
+      <c r="H5" s="26">
         <v>14.202880859375</v>
       </c>
-      <c r="I5" s="35">
+      <c r="I5" s="26">
         <v>42.7520751953125</v>
       </c>
-      <c r="J5" s="35">
+      <c r="J5" s="26">
         <v>89.6240234375</v>
       </c>
-      <c r="K5" s="35">
+      <c r="K5" s="26">
         <v>99.7467041015625</v>
       </c>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
       <c r="R5" s="15"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="28"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="3">
         <v>16</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35">
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26">
         <v>2.447509765625</v>
       </c>
-      <c r="H6" s="35">
+      <c r="H6" s="26">
         <v>3.5919189453125</v>
       </c>
-      <c r="I6" s="35">
+      <c r="I6" s="26">
         <v>6.94580078125</v>
       </c>
-      <c r="J6" s="35">
+      <c r="J6" s="26">
         <v>17.08984375</v>
       </c>
-      <c r="K6" s="35">
+      <c r="K6" s="26">
         <v>49.7650146484375</v>
       </c>
-      <c r="L6" s="35">
+      <c r="L6" s="26">
         <v>91.68701171875</v>
       </c>
-      <c r="M6" s="35">
+      <c r="M6" s="26">
         <v>99.6368408203125</v>
       </c>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
       <c r="R6" s="15"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="28"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="3">
         <v>32</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35">
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26">
         <v>2.0111083984375</v>
       </c>
-      <c r="I7" s="35">
+      <c r="I7" s="26">
         <v>2.8228759765625</v>
       </c>
-      <c r="J7" s="35">
+      <c r="J7" s="26">
         <v>4.193115234375</v>
       </c>
-      <c r="K7" s="35">
+      <c r="K7" s="26">
         <v>6.7291259765625</v>
       </c>
-      <c r="L7" s="35">
+      <c r="L7" s="26">
         <v>17.205810546875</v>
       </c>
-      <c r="M7" s="35">
+      <c r="M7" s="26">
         <v>50.9857177734375</v>
       </c>
-      <c r="N7" s="35">
+      <c r="N7" s="26">
         <v>92.626953125</v>
       </c>
-      <c r="O7" s="35">
+      <c r="O7" s="26">
         <v>99.969482421875</v>
       </c>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
       <c r="R7" s="15"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="28"/>
-      <c r="B8" s="31"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="3">
         <v>64</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35">
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26">
         <v>2.5604248046875</v>
       </c>
-      <c r="L8" s="35">
+      <c r="L8" s="26">
         <v>3.8818359375</v>
       </c>
-      <c r="M8" s="35">
+      <c r="M8" s="26">
         <v>7.0068359375</v>
       </c>
-      <c r="N8" s="35">
+      <c r="N8" s="26">
         <v>15.9454345703125</v>
       </c>
-      <c r="O8" s="35">
+      <c r="O8" s="26">
         <v>50.0518798828125</v>
       </c>
-      <c r="P8" s="35">
+      <c r="P8" s="26">
         <v>91.9647216796875</v>
       </c>
-      <c r="Q8" s="35">
+      <c r="Q8" s="26">
         <v>100</v>
       </c>
       <c r="R8" s="15"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="28"/>
-      <c r="B9" s="32"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="10">
         <v>128</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35">
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26">
         <v>2.703857421875</v>
       </c>
-      <c r="N9" s="35">
+      <c r="N9" s="26">
         <v>3.863525390625</v>
       </c>
-      <c r="O9" s="35">
+      <c r="O9" s="26">
         <v>7.0526123046875</v>
       </c>
-      <c r="P9" s="35">
+      <c r="P9" s="26">
         <v>16.436767578125</v>
       </c>
-      <c r="Q9" s="35">
+      <c r="Q9" s="26">
         <v>52.2705078125</v>
       </c>
       <c r="R9" s="15">
@@ -3502,8 +3502,8 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="28"/>
-      <c r="B10" s="33">
+      <c r="A10" s="31"/>
+      <c r="B10" s="37">
         <v>2</v>
       </c>
       <c r="C10" s="12">
@@ -3540,71 +3540,71 @@
       <c r="R10" s="16"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="28"/>
-      <c r="B11" s="31"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="3">
         <v>4</v>
       </c>
       <c r="D11" s="23"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35">
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26">
         <v>2.691650390625</v>
       </c>
-      <c r="K11" s="35">
+      <c r="K11" s="26">
         <v>3.9215087890625</v>
       </c>
-      <c r="L11" s="35">
+      <c r="L11" s="26">
         <v>6.524658203125</v>
       </c>
-      <c r="M11" s="35">
+      <c r="M11" s="26">
         <v>17.413330078125</v>
       </c>
-      <c r="N11" s="35">
+      <c r="N11" s="26">
         <v>50.994873046875</v>
       </c>
-      <c r="O11" s="35">
+      <c r="O11" s="26">
         <v>92.4224853515625</v>
       </c>
-      <c r="P11" s="35">
+      <c r="P11" s="26">
         <v>99.859619140625</v>
       </c>
-      <c r="Q11" s="35"/>
+      <c r="Q11" s="26"/>
       <c r="R11" s="15"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="28"/>
-      <c r="B12" s="31"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="3">
         <v>8</v>
       </c>
       <c r="D12" s="23"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35">
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26">
         <v>2.1240234375</v>
       </c>
-      <c r="M12" s="35">
+      <c r="M12" s="26">
         <v>2.9052734375</v>
       </c>
-      <c r="N12" s="35">
+      <c r="N12" s="26">
         <v>4.949951171875</v>
       </c>
-      <c r="O12" s="35">
+      <c r="O12" s="26">
         <v>9.0362548828125</v>
       </c>
-      <c r="P12" s="35">
+      <c r="P12" s="26">
         <v>25.47607421875</v>
       </c>
-      <c r="Q12" s="35">
+      <c r="Q12" s="26">
         <v>69.7113037109375</v>
       </c>
       <c r="R12" s="15">
@@ -3612,8 +3612,8 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
-      <c r="B13" s="32"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="10">
         <v>16</v>
       </c>
@@ -3640,33 +3640,33 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="28"/>
-      <c r="B14" s="31">
+      <c r="A14" s="31"/>
+      <c r="B14" s="35">
         <v>3</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35">
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26">
         <v>2.5054931640625</v>
       </c>
-      <c r="O14" s="35">
+      <c r="O14" s="26">
         <v>3.5491943359375</v>
       </c>
-      <c r="P14" s="35">
+      <c r="P14" s="26">
         <v>6.1920166015625</v>
       </c>
-      <c r="Q14" s="35">
+      <c r="Q14" s="26">
         <v>14.788818359375</v>
       </c>
       <c r="R14" s="15">
@@ -3674,8 +3674,8 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="29"/>
-      <c r="B15" s="34"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="4">
         <v>4</v>
       </c>
@@ -3702,10 +3702,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="38">
+      <c r="A16" s="32">
         <v>64</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="34">
         <v>1</v>
       </c>
       <c r="C16" s="5">
@@ -3740,199 +3740,199 @@
       <c r="R16" s="14"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17" s="28"/>
-      <c r="B17" s="31"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="3">
         <v>4</v>
       </c>
       <c r="D17" s="23"/>
-      <c r="E17" s="35">
+      <c r="E17" s="26">
         <v>2.0233154296875</v>
       </c>
-      <c r="F17" s="35">
+      <c r="F17" s="26">
         <v>3.77044677734375</v>
       </c>
-      <c r="G17" s="35">
+      <c r="G17" s="26">
         <v>8.75396728515625</v>
       </c>
-      <c r="H17" s="35">
+      <c r="H17" s="26">
         <v>33.0062866210937</v>
       </c>
-      <c r="I17" s="35">
+      <c r="I17" s="26">
         <v>86.845397949218693</v>
       </c>
-      <c r="J17" s="35">
+      <c r="J17" s="26">
         <v>99.894714355468693</v>
       </c>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
       <c r="R17" s="15"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18" s="28"/>
-      <c r="B18" s="31"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="3">
         <v>8</v>
       </c>
       <c r="D18" s="23"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35">
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26">
         <v>3.00445556640625</v>
       </c>
-      <c r="H18" s="35">
+      <c r="H18" s="26">
         <v>6.37969970703125</v>
       </c>
-      <c r="I18" s="35">
+      <c r="I18" s="26">
         <v>20.0759887695312</v>
       </c>
-      <c r="J18" s="35">
+      <c r="J18" s="26">
         <v>71.189880371093693</v>
       </c>
-      <c r="K18" s="35">
+      <c r="K18" s="26">
         <v>98.7518310546875</v>
       </c>
-      <c r="L18" s="35">
+      <c r="L18" s="26">
         <v>100</v>
       </c>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="26"/>
       <c r="R18" s="15"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A19" s="28"/>
-      <c r="B19" s="31"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="3">
         <v>16</v>
       </c>
       <c r="D19" s="23"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35">
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26">
         <v>3.23333740234375</v>
       </c>
-      <c r="J19" s="35">
+      <c r="J19" s="26">
         <v>7.74993896484375</v>
       </c>
-      <c r="K19" s="35">
+      <c r="K19" s="26">
         <v>27.1514892578125</v>
       </c>
-      <c r="L19" s="35">
+      <c r="L19" s="26">
         <v>82.270812988281193</v>
       </c>
-      <c r="M19" s="35">
+      <c r="M19" s="26">
         <v>99.815368652343693</v>
       </c>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
       <c r="R19" s="15"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A20" s="28"/>
-      <c r="B20" s="31"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="3">
         <v>32</v>
       </c>
       <c r="D20" s="23"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35">
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26">
         <v>2.02484130859375</v>
       </c>
-      <c r="K20" s="35">
+      <c r="K20" s="26">
         <v>3.41796875</v>
       </c>
-      <c r="L20" s="35">
+      <c r="L20" s="26">
         <v>8.49609375</v>
       </c>
-      <c r="M20" s="35">
+      <c r="M20" s="26">
         <v>31.451416015625</v>
       </c>
-      <c r="N20" s="35">
+      <c r="N20" s="26">
         <v>84.4024658203125</v>
       </c>
-      <c r="O20" s="35">
+      <c r="O20" s="26">
         <v>99.853515625</v>
       </c>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="26"/>
       <c r="R20" s="15"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A21" s="28"/>
-      <c r="B21" s="31"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="3">
         <v>64</v>
       </c>
       <c r="D21" s="23"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35">
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26">
         <v>2.04925537109375</v>
       </c>
-      <c r="M21" s="35">
+      <c r="M21" s="26">
         <v>3.6529541015625</v>
       </c>
-      <c r="N21" s="35">
+      <c r="N21" s="26">
         <v>8.75244140625</v>
       </c>
-      <c r="O21" s="35">
+      <c r="O21" s="26">
         <v>30.7830810546875</v>
       </c>
-      <c r="P21" s="35">
+      <c r="P21" s="26">
         <v>85.807800292968693</v>
       </c>
-      <c r="Q21" s="35">
+      <c r="Q21" s="26">
         <v>99.71923828125</v>
       </c>
       <c r="R21" s="15"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A22" s="28"/>
-      <c r="B22" s="32"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="10">
         <v>128</v>
       </c>
       <c r="D22" s="23"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35">
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26">
         <v>2.07366943359375</v>
       </c>
-      <c r="O22" s="35">
+      <c r="O22" s="26">
         <v>3.5797119140625</v>
       </c>
-      <c r="P22" s="35">
+      <c r="P22" s="26">
         <v>8.46710205078125</v>
       </c>
-      <c r="Q22" s="35">
+      <c r="Q22" s="26">
         <v>32.0358276367187</v>
       </c>
       <c r="R22" s="15">
@@ -3940,8 +3940,8 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A23" s="28"/>
-      <c r="B23" s="33">
+      <c r="A23" s="31"/>
+      <c r="B23" s="37">
         <v>2</v>
       </c>
       <c r="C23" s="12">
@@ -3976,61 +3976,61 @@
       <c r="R23" s="16"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
-      <c r="B24" s="31"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="3">
         <v>4</v>
       </c>
       <c r="D24" s="23"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35">
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26">
         <v>3.27911376953125</v>
       </c>
-      <c r="N24" s="35">
+      <c r="N24" s="26">
         <v>7.06634521484375</v>
       </c>
-      <c r="O24" s="35">
+      <c r="O24" s="26">
         <v>25.1327514648437</v>
       </c>
-      <c r="P24" s="35">
+      <c r="P24" s="26">
         <v>78.376770019531193</v>
       </c>
-      <c r="Q24" s="35">
+      <c r="Q24" s="26">
         <v>99.473571777343693</v>
       </c>
       <c r="R24" s="15"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A25" s="28"/>
-      <c r="B25" s="31"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="3">
         <v>8</v>
       </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="35">
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26">
         <v>3.3111572265625</v>
       </c>
-      <c r="P25" s="35">
+      <c r="P25" s="26">
         <v>7.3974609375</v>
       </c>
-      <c r="Q25" s="35">
+      <c r="Q25" s="26">
         <v>25.23193359375</v>
       </c>
       <c r="R25" s="15">
@@ -4038,8 +4038,8 @@
       </c>
     </row>
     <row r="26" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="29"/>
-      <c r="B26" s="34"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="38"/>
       <c r="C26" s="4">
         <v>16</v>
       </c>
@@ -4101,23 +4101,23 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="27"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="30"/>
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
@@ -4176,251 +4176,251 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="28">
+      <c r="A3" s="31">
         <v>32</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="34">
         <v>1</v>
       </c>
       <c r="C3" s="5">
         <v>0</v>
       </c>
-      <c r="D3" s="35">
-        <v>0</v>
-      </c>
-      <c r="E3" s="35">
+      <c r="D3" s="26">
+        <v>0</v>
+      </c>
+      <c r="E3" s="26">
         <v>9.765625E-2</v>
       </c>
-      <c r="F3" s="35">
+      <c r="F3" s="26">
         <v>29.1015625</v>
       </c>
-      <c r="G3" s="35">
+      <c r="G3" s="26">
         <v>87.3046875</v>
       </c>
-      <c r="H3" s="35">
+      <c r="H3" s="26">
         <v>100</v>
       </c>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
       <c r="R3" s="15"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="28"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="3">
         <v>4</v>
       </c>
-      <c r="D4" s="35">
-        <v>0</v>
-      </c>
-      <c r="E4" s="35">
-        <v>0</v>
-      </c>
-      <c r="F4" s="35">
-        <v>0</v>
-      </c>
-      <c r="G4" s="35">
+      <c r="D4" s="26">
+        <v>0</v>
+      </c>
+      <c r="E4" s="26">
+        <v>0</v>
+      </c>
+      <c r="F4" s="26">
+        <v>0</v>
+      </c>
+      <c r="G4" s="26">
         <v>4.1015625</v>
       </c>
-      <c r="H4" s="35">
+      <c r="H4" s="26">
         <v>53.41796875</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="26">
         <v>97.55859375</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4" s="26">
         <v>100</v>
       </c>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
       <c r="R4" s="15"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="28"/>
-      <c r="B5" s="31"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="3">
         <v>8</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35">
-        <v>0</v>
-      </c>
-      <c r="F5" s="35">
-        <v>0</v>
-      </c>
-      <c r="G5" s="35">
-        <v>0</v>
-      </c>
-      <c r="H5" s="35">
+      <c r="D5" s="26"/>
+      <c r="E5" s="26">
+        <v>0</v>
+      </c>
+      <c r="F5" s="26">
+        <v>0</v>
+      </c>
+      <c r="G5" s="26">
+        <v>0</v>
+      </c>
+      <c r="H5" s="26">
         <v>0.390625</v>
       </c>
-      <c r="I5" s="35">
+      <c r="I5" s="26">
         <v>15.33203125</v>
       </c>
-      <c r="J5" s="35">
+      <c r="J5" s="26">
         <v>80.2734375</v>
       </c>
-      <c r="K5" s="35">
+      <c r="K5" s="26">
         <v>99.609375</v>
       </c>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
       <c r="R5" s="15"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="28"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="3">
         <v>16</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35">
-        <v>0</v>
-      </c>
-      <c r="H6" s="35">
-        <v>0</v>
-      </c>
-      <c r="I6" s="35">
-        <v>0</v>
-      </c>
-      <c r="J6" s="35">
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26">
+        <v>0</v>
+      </c>
+      <c r="H6" s="26">
+        <v>0</v>
+      </c>
+      <c r="I6" s="26">
+        <v>0</v>
+      </c>
+      <c r="J6" s="26">
         <v>0.78125</v>
       </c>
-      <c r="K6" s="35">
+      <c r="K6" s="26">
         <v>22.94921875</v>
       </c>
-      <c r="L6" s="35">
+      <c r="L6" s="26">
         <v>84.86328125</v>
       </c>
-      <c r="M6" s="35">
+      <c r="M6" s="26">
         <v>99.4140625</v>
       </c>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
       <c r="R6" s="15"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="28"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="3">
         <v>32</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35">
-        <v>0</v>
-      </c>
-      <c r="I7" s="35">
-        <v>0</v>
-      </c>
-      <c r="J7" s="35">
-        <v>0</v>
-      </c>
-      <c r="K7" s="35">
-        <v>0</v>
-      </c>
-      <c r="L7" s="35">
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26">
+        <v>0</v>
+      </c>
+      <c r="I7" s="26">
+        <v>0</v>
+      </c>
+      <c r="J7" s="26">
+        <v>0</v>
+      </c>
+      <c r="K7" s="26">
+        <v>0</v>
+      </c>
+      <c r="L7" s="26">
         <v>0.48828125</v>
       </c>
-      <c r="M7" s="35">
+      <c r="M7" s="26">
         <v>24.0234375</v>
       </c>
-      <c r="N7" s="35">
+      <c r="N7" s="26">
         <v>86.328125</v>
       </c>
-      <c r="O7" s="35">
+      <c r="O7" s="26">
         <v>99.90234375</v>
       </c>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
       <c r="R7" s="15"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="28"/>
-      <c r="B8" s="31"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="3">
         <v>64</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35">
-        <v>0</v>
-      </c>
-      <c r="L8" s="35">
-        <v>0</v>
-      </c>
-      <c r="M8" s="35">
-        <v>0</v>
-      </c>
-      <c r="N8" s="35">
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26">
+        <v>0</v>
+      </c>
+      <c r="L8" s="26">
+        <v>0</v>
+      </c>
+      <c r="M8" s="26">
+        <v>0</v>
+      </c>
+      <c r="N8" s="26">
         <v>0.390625</v>
       </c>
-      <c r="O8" s="35">
+      <c r="O8" s="26">
         <v>24.12109375</v>
       </c>
-      <c r="P8" s="35">
+      <c r="P8" s="26">
         <v>85.64453125</v>
       </c>
-      <c r="Q8" s="35">
+      <c r="Q8" s="26">
         <v>100</v>
       </c>
       <c r="R8" s="15"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="28"/>
-      <c r="B9" s="31"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="3">
         <v>128</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35">
-        <v>0</v>
-      </c>
-      <c r="N9" s="35">
-        <v>0</v>
-      </c>
-      <c r="O9" s="35">
-        <v>0</v>
-      </c>
-      <c r="P9" s="35">
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26">
+        <v>0</v>
+      </c>
+      <c r="N9" s="26">
+        <v>0</v>
+      </c>
+      <c r="O9" s="26">
+        <v>0</v>
+      </c>
+      <c r="P9" s="26">
         <v>0.78125</v>
       </c>
-      <c r="Q9" s="35">
+      <c r="Q9" s="26">
         <v>25.29296875</v>
       </c>
       <c r="R9" s="15">
@@ -4428,8 +4428,8 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="28"/>
-      <c r="B10" s="33">
+      <c r="A10" s="31"/>
+      <c r="B10" s="37">
         <v>2</v>
       </c>
       <c r="C10" s="12">
@@ -4466,71 +4466,71 @@
       <c r="R10" s="16"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="28"/>
-      <c r="B11" s="31"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="3">
         <v>4</v>
       </c>
       <c r="D11" s="23"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35">
-        <v>0</v>
-      </c>
-      <c r="K11" s="35">
-        <v>0</v>
-      </c>
-      <c r="L11" s="35">
-        <v>0</v>
-      </c>
-      <c r="M11" s="35">
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26">
+        <v>0</v>
+      </c>
+      <c r="K11" s="26">
+        <v>0</v>
+      </c>
+      <c r="L11" s="26">
+        <v>0</v>
+      </c>
+      <c r="M11" s="26">
         <v>0.390625</v>
       </c>
-      <c r="N11" s="35">
+      <c r="N11" s="26">
         <v>23.828125</v>
       </c>
-      <c r="O11" s="35">
+      <c r="O11" s="26">
         <v>85.7421875</v>
       </c>
-      <c r="P11" s="35">
+      <c r="P11" s="26">
         <v>99.8046875</v>
       </c>
-      <c r="Q11" s="35"/>
+      <c r="Q11" s="26"/>
       <c r="R11" s="15"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="28"/>
-      <c r="B12" s="31"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="3">
         <v>8</v>
       </c>
       <c r="D12" s="23"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35">
-        <v>0</v>
-      </c>
-      <c r="M12" s="35">
-        <v>0</v>
-      </c>
-      <c r="N12" s="35">
-        <v>0</v>
-      </c>
-      <c r="O12" s="35">
-        <v>0</v>
-      </c>
-      <c r="P12" s="35">
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26">
+        <v>0</v>
+      </c>
+      <c r="M12" s="26">
+        <v>0</v>
+      </c>
+      <c r="N12" s="26">
+        <v>0</v>
+      </c>
+      <c r="O12" s="26">
+        <v>0</v>
+      </c>
+      <c r="P12" s="26">
         <v>3.22265625</v>
       </c>
-      <c r="Q12" s="35">
+      <c r="Q12" s="26">
         <v>47.265625</v>
       </c>
       <c r="R12" s="15">
@@ -4538,8 +4538,8 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
-      <c r="B13" s="32"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="10">
         <v>16</v>
       </c>
@@ -4566,33 +4566,33 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="28"/>
-      <c r="B14" s="31">
+      <c r="A14" s="31"/>
+      <c r="B14" s="35">
         <v>3</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35">
-        <v>0</v>
-      </c>
-      <c r="O14" s="35">
-        <v>0</v>
-      </c>
-      <c r="P14" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="35">
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26">
+        <v>0</v>
+      </c>
+      <c r="O14" s="26">
+        <v>0</v>
+      </c>
+      <c r="P14" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="26">
         <v>0.1953125</v>
       </c>
       <c r="R14" s="15">
@@ -4600,8 +4600,8 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="29"/>
-      <c r="B15" s="34"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="4">
         <v>4</v>
       </c>
@@ -4628,10 +4628,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="38">
+      <c r="A16" s="32">
         <v>64</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="34">
         <v>1</v>
       </c>
       <c r="C16" s="5">
@@ -4666,199 +4666,199 @@
       <c r="R16" s="14"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17" s="28"/>
-      <c r="B17" s="31"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="3">
         <v>4</v>
       </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35">
-        <v>0</v>
-      </c>
-      <c r="F17" s="35">
-        <v>0</v>
-      </c>
-      <c r="G17" s="35">
-        <v>0</v>
-      </c>
-      <c r="H17" s="35">
+      <c r="D17" s="26"/>
+      <c r="E17" s="26">
+        <v>0</v>
+      </c>
+      <c r="F17" s="26">
+        <v>0</v>
+      </c>
+      <c r="G17" s="26">
+        <v>0</v>
+      </c>
+      <c r="H17" s="26">
         <v>6.0546875</v>
       </c>
-      <c r="I17" s="35">
+      <c r="I17" s="26">
         <v>75.78125</v>
       </c>
-      <c r="J17" s="35">
+      <c r="J17" s="26">
         <v>99.8046875</v>
       </c>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
       <c r="R17" s="15"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18" s="28"/>
-      <c r="B18" s="31"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="3">
         <v>8</v>
       </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35">
-        <v>0</v>
-      </c>
-      <c r="H18" s="35">
-        <v>0</v>
-      </c>
-      <c r="I18" s="35">
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26">
+        <v>0</v>
+      </c>
+      <c r="H18" s="26">
+        <v>0</v>
+      </c>
+      <c r="I18" s="26">
         <v>1.5625</v>
       </c>
-      <c r="J18" s="35">
+      <c r="J18" s="26">
         <v>50.48828125</v>
       </c>
-      <c r="K18" s="35">
+      <c r="K18" s="26">
         <v>97.65625</v>
       </c>
-      <c r="L18" s="35">
+      <c r="L18" s="26">
         <v>100</v>
       </c>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="26"/>
       <c r="R18" s="15"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A19" s="28"/>
-      <c r="B19" s="31"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="3">
         <v>16</v>
       </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35">
-        <v>0</v>
-      </c>
-      <c r="J19" s="35">
-        <v>0</v>
-      </c>
-      <c r="K19" s="35">
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26">
+        <v>0</v>
+      </c>
+      <c r="J19" s="26">
+        <v>0</v>
+      </c>
+      <c r="K19" s="26">
         <v>3.80859375</v>
       </c>
-      <c r="L19" s="35">
+      <c r="L19" s="26">
         <v>68.75</v>
       </c>
-      <c r="M19" s="35">
+      <c r="M19" s="26">
         <v>99.51171875</v>
       </c>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
       <c r="R19" s="15"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A20" s="28"/>
-      <c r="B20" s="31"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="3">
         <v>32</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35">
-        <v>0</v>
-      </c>
-      <c r="K20" s="35">
-        <v>0</v>
-      </c>
-      <c r="L20" s="35">
-        <v>0</v>
-      </c>
-      <c r="M20" s="35">
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26">
+        <v>0</v>
+      </c>
+      <c r="K20" s="26">
+        <v>0</v>
+      </c>
+      <c r="L20" s="26">
+        <v>0</v>
+      </c>
+      <c r="M20" s="26">
         <v>5.76171875</v>
       </c>
-      <c r="N20" s="35">
+      <c r="N20" s="26">
         <v>72.0703125</v>
       </c>
-      <c r="O20" s="35">
+      <c r="O20" s="26">
         <v>99.70703125</v>
       </c>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="26"/>
       <c r="R20" s="15"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A21" s="28"/>
-      <c r="B21" s="31"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="3">
         <v>64</v>
       </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35">
-        <v>0</v>
-      </c>
-      <c r="M21" s="35">
-        <v>0</v>
-      </c>
-      <c r="N21" s="35">
-        <v>0</v>
-      </c>
-      <c r="O21" s="35">
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26">
+        <v>0</v>
+      </c>
+      <c r="M21" s="26">
+        <v>0</v>
+      </c>
+      <c r="N21" s="26">
+        <v>0</v>
+      </c>
+      <c r="O21" s="26">
         <v>5.46875</v>
       </c>
-      <c r="P21" s="35">
+      <c r="P21" s="26">
         <v>74.51171875</v>
       </c>
-      <c r="Q21" s="35">
+      <c r="Q21" s="26">
         <v>99.51171875</v>
       </c>
       <c r="R21" s="15"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A22" s="28"/>
-      <c r="B22" s="31"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="3">
         <v>128</v>
       </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35">
-        <v>0</v>
-      </c>
-      <c r="O22" s="35">
-        <v>0</v>
-      </c>
-      <c r="P22" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="35">
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26">
+        <v>0</v>
+      </c>
+      <c r="O22" s="26">
+        <v>0</v>
+      </c>
+      <c r="P22" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="26">
         <v>6.0546875</v>
       </c>
       <c r="R22" s="15">
@@ -4866,8 +4866,8 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A23" s="28"/>
-      <c r="B23" s="33">
+      <c r="A23" s="31"/>
+      <c r="B23" s="37">
         <v>2</v>
       </c>
       <c r="C23" s="12">
@@ -4902,61 +4902,61 @@
       <c r="R23" s="16"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
-      <c r="B24" s="31"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="3">
         <v>4</v>
       </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35">
-        <v>0</v>
-      </c>
-      <c r="N24" s="35">
-        <v>0</v>
-      </c>
-      <c r="O24" s="35">
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26">
+        <v>0</v>
+      </c>
+      <c r="N24" s="26">
+        <v>0</v>
+      </c>
+      <c r="O24" s="26">
         <v>2.5390625</v>
       </c>
-      <c r="P24" s="35">
+      <c r="P24" s="26">
         <v>62.109375</v>
       </c>
-      <c r="Q24" s="35">
+      <c r="Q24" s="26">
         <v>99.0234375</v>
       </c>
       <c r="R24" s="15"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A25" s="28"/>
-      <c r="B25" s="31"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="3">
         <v>8</v>
       </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="35">
-        <v>0</v>
-      </c>
-      <c r="P25" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="35">
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26">
+        <v>0</v>
+      </c>
+      <c r="P25" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="26">
         <v>2.34375</v>
       </c>
       <c r="R25" s="15">
@@ -4964,7 +4964,7 @@
       </c>
     </row>
     <row r="26" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="29"/>
+      <c r="A26" s="33"/>
       <c r="B26" s="11">
         <v>3</v>
       </c>

</xml_diff>